<commit_message>
ft: removed position cuts
</commit_message>
<xml_diff>
--- a/data/campeonato_4_1.xlsx
+++ b/data/campeonato_4_1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="26">
   <si>
     <t>EQUIPO</t>
   </si>
@@ -59,37 +59,40 @@
     <t>1/1/2022</t>
   </si>
   <si>
-    <t>4:4</t>
-  </si>
-  <si>
-    <t>2:4</t>
+    <t>2:3</t>
+  </si>
+  <si>
+    <t>1:5</t>
+  </si>
+  <si>
+    <t>6:4</t>
+  </si>
+  <si>
+    <t>0:2</t>
+  </si>
+  <si>
+    <t>1:4</t>
   </si>
   <si>
     <t>3:2</t>
   </si>
   <si>
-    <t>2:7</t>
-  </si>
-  <si>
-    <t>2:3</t>
-  </si>
-  <si>
-    <t>5:1</t>
+    <t>0:6</t>
+  </si>
+  <si>
+    <t>2:2</t>
+  </si>
+  <si>
+    <t>5:4</t>
+  </si>
+  <si>
+    <t>1:0</t>
+  </si>
+  <si>
+    <t>3:4</t>
   </si>
   <si>
     <t>3:1</t>
-  </si>
-  <si>
-    <t>2:0</t>
-  </si>
-  <si>
-    <t>3:4</t>
-  </si>
-  <si>
-    <t>0:2</t>
-  </si>
-  <si>
-    <t>4:2</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,7 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -469,7 +472,7 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -486,7 +489,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -503,7 +506,7 @@
         <v>7</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -582,10 +585,10 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
@@ -596,10 +599,10 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
@@ -621,7 +624,7 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -635,7 +638,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -654,7 +657,7 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -668,7 +671,7 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -687,7 +690,7 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -701,7 +704,7 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -720,7 +723,7 @@
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -734,7 +737,7 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>